<commit_message>
Created a test bar chart for missing values in D3
</commit_message>
<xml_diff>
--- a/Project supporting Artifacts/Feature requirements/DataPolish_Features.xlsx
+++ b/Project supporting Artifacts/Feature requirements/DataPolish_Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seanmccrossan/group_project/TUD-Group-Project/Project supporting Artifacts/Feature requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9537FBB-291C-6E4A-8ABC-45CA4718A07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92C879E-0070-0D48-83BF-5FDCBD0DDA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20500" activeTab="1" xr2:uid="{6E789A33-B115-BE41-929D-FD6EA5DE1201}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sub level features" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sub level features'!$B$3:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sub level features'!$B$3:$H$60</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1251,9 +1251,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1267,15 +1264,18 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1608,14 +1608,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
@@ -1952,7 +1952,7 @@
   <dimension ref="A2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1966,63 +1966,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="40" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>178</v>
       </c>
-      <c r="F2" s="49" t="s">
+      <c r="F2" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="47" t="s">
         <v>221</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="K2" s="48" t="s">
+      <c r="K2" s="47" t="s">
         <v>228</v>
       </c>
-      <c r="L2" s="48" t="s">
+      <c r="L2" s="47" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="44">
+      <c r="A3" s="43">
         <v>2</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="43" t="s">
         <v>179</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="44" t="s">
         <v>203</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3" s="51">
+      <c r="G3" s="50">
         <v>45194</v>
       </c>
-      <c r="H3" s="51">
+      <c r="H3" s="50">
         <v>45200</v>
       </c>
-      <c r="I3" s="50">
+      <c r="I3" s="49">
         <v>5</v>
       </c>
       <c r="J3" t="s">
@@ -2036,28 +2036,28 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A4" s="44">
+      <c r="A4" s="43">
         <v>3</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="44" t="s">
         <v>204</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4" s="51">
+      <c r="G4" s="50">
         <v>45194</v>
       </c>
-      <c r="H4" s="51">
+      <c r="H4" s="50">
         <v>45207</v>
       </c>
-      <c r="I4" s="50">
+      <c r="I4" s="49">
         <v>10</v>
       </c>
       <c r="J4" t="s">
@@ -2071,25 +2071,25 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A5" s="44">
+      <c r="A5" s="43">
         <v>4</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="D5" s="45" t="s">
+      <c r="D5" s="44" t="s">
         <v>205</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5" s="51">
+      <c r="G5" s="50">
         <v>45194</v>
       </c>
-      <c r="H5" s="51">
+      <c r="H5" s="50">
         <v>45228</v>
       </c>
       <c r="I5">
@@ -2106,25 +2106,25 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A6" s="44">
+      <c r="A6" s="43">
         <v>5</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="C6" s="44" t="s">
+      <c r="C6" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="44" t="s">
         <v>206</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6" s="51">
+      <c r="G6" s="50">
         <v>45194</v>
       </c>
-      <c r="H6" s="51">
+      <c r="H6" s="50">
         <v>45228</v>
       </c>
       <c r="I6">
@@ -2141,25 +2141,25 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="44">
+      <c r="A7" s="43">
         <v>6</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="44" t="s">
         <v>196</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="44" t="s">
         <v>207</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7" s="51">
+      <c r="G7" s="50">
         <v>45194</v>
       </c>
-      <c r="H7" s="51">
+      <c r="H7" s="50">
         <v>45228</v>
       </c>
       <c r="I7">
@@ -2176,25 +2176,25 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A8" s="42">
+      <c r="A8" s="41">
         <v>7</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="42" t="s">
         <v>197</v>
       </c>
-      <c r="D8" s="43" t="s">
+      <c r="D8" s="42" t="s">
         <v>208</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="51">
         <v>45201</v>
       </c>
-      <c r="H8" s="51">
+      <c r="H8" s="50">
         <v>45207</v>
       </c>
       <c r="I8">
@@ -2211,25 +2211,25 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A9" s="42">
+      <c r="A9" s="41">
         <v>8</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="42" t="s">
         <v>209</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="51">
         <v>45201</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="50">
         <v>45207</v>
       </c>
       <c r="I9">
@@ -2246,25 +2246,25 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A10" s="42">
+      <c r="A10" s="41">
         <v>9</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="42" t="s">
         <v>210</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="51">
         <v>45208</v>
       </c>
-      <c r="H10" s="51">
+      <c r="H10" s="50">
         <v>45212</v>
       </c>
       <c r="I10">
@@ -2281,25 +2281,25 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A11" s="42">
+      <c r="A11" s="41">
         <v>10</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="42" t="s">
         <v>200</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="42" t="s">
         <v>211</v>
       </c>
       <c r="F11">
         <v>4</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="51">
         <v>45208</v>
       </c>
-      <c r="H11" s="51">
+      <c r="H11" s="50">
         <v>45221</v>
       </c>
       <c r="I11">
@@ -2316,25 +2316,25 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="42">
+      <c r="A12" s="41">
         <v>11</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="42" t="s">
         <v>212</v>
       </c>
       <c r="F12">
         <v>5</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G12" s="51">
         <v>45215</v>
       </c>
-      <c r="H12" s="51">
+      <c r="H12" s="50">
         <v>45221</v>
       </c>
       <c r="I12">
@@ -2351,25 +2351,25 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A13" s="46">
+      <c r="A13" s="45">
         <v>12</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="45" t="s">
         <v>189</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="46" t="s">
         <v>213</v>
       </c>
       <c r="F13">
         <v>6</v>
       </c>
-      <c r="G13" s="52">
+      <c r="G13" s="51">
         <v>45222</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="50">
         <v>45228</v>
       </c>
       <c r="I13">
@@ -2386,25 +2386,25 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="46">
+      <c r="A14" s="45">
         <v>13</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="45" t="s">
         <v>190</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="46" t="s">
         <v>214</v>
       </c>
       <c r="F14">
         <v>7</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="52">
         <v>45229</v>
       </c>
-      <c r="H14" s="54">
+      <c r="H14" s="53">
         <v>45235</v>
       </c>
       <c r="I14">
@@ -2421,25 +2421,25 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="27" x14ac:dyDescent="0.2">
-      <c r="A15" s="46">
+      <c r="A15" s="45">
         <v>14</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="46" t="s">
         <v>215</v>
       </c>
       <c r="F15">
         <v>7</v>
       </c>
-      <c r="G15" s="53">
+      <c r="G15" s="52">
         <v>45229</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H15" s="53">
         <v>45235</v>
       </c>
       <c r="I15">
@@ -2459,10 +2459,10 @@
       <c r="F16">
         <v>7</v>
       </c>
-      <c r="G16" s="53">
+      <c r="G16" s="52">
         <v>45229</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H16" s="53">
         <v>45242</v>
       </c>
       <c r="I16">
@@ -2482,10 +2482,10 @@
       <c r="F17">
         <v>7</v>
       </c>
-      <c r="G17" s="53">
+      <c r="G17" s="52">
         <v>45229</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="53">
         <v>45242</v>
       </c>
       <c r="I17">
@@ -2505,10 +2505,10 @@
       <c r="F18">
         <v>7</v>
       </c>
-      <c r="G18" s="53">
+      <c r="G18" s="52">
         <v>45229</v>
       </c>
-      <c r="H18" s="54">
+      <c r="H18" s="53">
         <v>45242</v>
       </c>
       <c r="I18">
@@ -2528,10 +2528,10 @@
       <c r="F19">
         <v>8</v>
       </c>
-      <c r="G19" s="55">
+      <c r="G19" s="54">
         <v>45236</v>
       </c>
-      <c r="H19" s="54">
+      <c r="H19" s="53">
         <v>45242</v>
       </c>
       <c r="I19">
@@ -2551,10 +2551,10 @@
       <c r="F20">
         <v>9</v>
       </c>
-      <c r="G20" s="53">
+      <c r="G20" s="52">
         <v>45243</v>
       </c>
-      <c r="H20" s="54">
+      <c r="H20" s="53">
         <v>45249</v>
       </c>
       <c r="I20">
@@ -2574,10 +2574,10 @@
       <c r="F21">
         <v>9</v>
       </c>
-      <c r="G21" s="53">
+      <c r="G21" s="52">
         <v>45243</v>
       </c>
-      <c r="H21" s="54">
+      <c r="H21" s="53">
         <v>45256</v>
       </c>
       <c r="I21">
@@ -2597,10 +2597,10 @@
       <c r="F22">
         <v>9</v>
       </c>
-      <c r="G22" s="53">
+      <c r="G22" s="52">
         <v>45243</v>
       </c>
-      <c r="H22" s="54">
+      <c r="H22" s="53">
         <v>45256</v>
       </c>
       <c r="I22">
@@ -2617,10 +2617,10 @@
       </c>
     </row>
     <row r="23" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G23" s="56">
+      <c r="G23" s="55">
         <v>45257</v>
       </c>
-      <c r="H23" s="56">
+      <c r="H23" s="55">
         <v>45277</v>
       </c>
       <c r="I23">
@@ -2637,10 +2637,10 @@
       </c>
     </row>
     <row r="24" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G24" s="56">
+      <c r="G24" s="55">
         <v>45257</v>
       </c>
-      <c r="H24" s="56">
+      <c r="H24" s="55">
         <v>45277</v>
       </c>
       <c r="I24">
@@ -2657,10 +2657,10 @@
       </c>
     </row>
     <row r="25" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G25" s="56">
+      <c r="G25" s="55">
         <v>45257</v>
       </c>
-      <c r="H25" s="56">
+      <c r="H25" s="55">
         <v>45277</v>
       </c>
       <c r="I25">
@@ -2677,10 +2677,10 @@
       </c>
     </row>
     <row r="26" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G26" s="56">
+      <c r="G26" s="55">
         <v>45278</v>
       </c>
-      <c r="H26" s="56">
+      <c r="H26" s="55">
         <v>45284</v>
       </c>
       <c r="I26">
@@ -2697,10 +2697,10 @@
       </c>
     </row>
     <row r="27" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="G27" s="56">
+      <c r="G27" s="55">
         <v>45278</v>
       </c>
-      <c r="H27" s="56">
+      <c r="H27" s="55">
         <v>45284</v>
       </c>
       <c r="I27">
@@ -2723,10 +2723,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B12DF85-055B-7B43-90A4-588AD8B6740D}">
+  <sheetPr filterMode="1"/>
   <dimension ref="B2:H62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2740,15 +2741,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
     </row>
     <row r="3" spans="2:8" ht="35" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -2773,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2796,7 +2797,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
@@ -2819,7 +2820,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2842,7 +2843,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
@@ -2888,7 +2889,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" s="20" t="s">
         <v>20</v>
       </c>
@@ -2911,7 +2912,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
         <v>20</v>
       </c>
@@ -2934,7 +2935,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="s">
         <v>20</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
         <v>20</v>
       </c>
@@ -2980,7 +2981,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="20" t="s">
         <v>20</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
         <v>20</v>
       </c>
@@ -3026,7 +3027,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="20" t="s">
         <v>20</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" s="20" t="s">
         <v>20</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="s">
         <v>20</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20" t="s">
         <v>20</v>
       </c>
@@ -3118,7 +3119,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" s="20" t="s">
         <v>20</v>
       </c>
@@ -3141,7 +3142,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" s="20" t="s">
         <v>53</v>
       </c>
@@ -3164,7 +3165,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" s="20" t="s">
         <v>53</v>
       </c>
@@ -3187,7 +3188,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="20" t="s">
         <v>53</v>
       </c>
@@ -3210,7 +3211,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="20" t="s">
         <v>53</v>
       </c>
@@ -3233,7 +3234,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="20" t="s">
         <v>53</v>
       </c>
@@ -3256,7 +3257,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
         <v>53</v>
       </c>
@@ -3279,7 +3280,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="s">
         <v>53</v>
       </c>
@@ -3302,7 +3303,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="s">
         <v>53</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
         <v>53</v>
       </c>
@@ -3348,7 +3349,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="20" t="s">
         <v>53</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="20" t="s">
         <v>53</v>
       </c>
@@ -3394,7 +3395,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="20" t="s">
         <v>53</v>
       </c>
@@ -3417,7 +3418,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="32" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="20" t="s">
         <v>53</v>
       </c>
@@ -3601,7 +3602,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" s="20" t="s">
         <v>103</v>
       </c>
@@ -3624,7 +3625,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="20" t="s">
         <v>103</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" s="20" t="s">
         <v>103</v>
       </c>
@@ -3670,7 +3671,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>77</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>77</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>77</v>
       </c>
@@ -3739,7 +3740,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>111</v>
       </c>
@@ -3762,7 +3763,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
         <v>111</v>
       </c>
@@ -3785,7 +3786,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>111</v>
       </c>
@@ -3808,7 +3809,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:8" ht="35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>111</v>
       </c>
@@ -3831,7 +3832,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="2:8" ht="85" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:8" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
         <v>120</v>
       </c>
@@ -3854,7 +3855,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="85" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:8" ht="85" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" s="20" t="s">
         <v>127</v>
       </c>
@@ -3877,7 +3878,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" s="20" t="s">
         <v>127</v>
       </c>
@@ -3900,7 +3901,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" s="20" t="s">
         <v>133</v>
       </c>
@@ -3923,7 +3924,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" s="20" t="s">
         <v>133</v>
       </c>
@@ -3946,7 +3947,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" s="26" t="s">
         <v>133</v>
       </c>
@@ -3969,7 +3970,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>141</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="2:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:8" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" s="21" t="s">
         <v>141</v>
       </c>
@@ -4015,7 +4016,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:8" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" s="20" t="s">
         <v>148</v>
       </c>
@@ -4036,7 +4037,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" s="20" t="s">
         <v>147</v>
       </c>
@@ -4057,7 +4058,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:8" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>124</v>
       </c>
@@ -4091,7 +4092,13 @@
     </row>
     <row r="62" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="B3:H3" xr:uid="{5B12DF85-055B-7B43-90A4-588AD8B6740D}"/>
+  <autoFilter ref="B3:H60" xr:uid="{5B12DF85-055B-7B43-90A4-588AD8B6740D}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Interactive data profile dashboard V2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
   </mergeCells>

</xml_diff>